<commit_message>
add results lia-sinequa for se2-aw
</commit_message>
<xml_diff>
--- a/trends/WSD state of the art.xlsx
+++ b/trends/WSD state of the art.xlsx
@@ -13,14 +13,14 @@
     <sheet state="visible" name="ideas" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">results!$A$1:$S$96</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">results!$A$1:$S$97</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="186">
   <si>
     <t>described</t>
   </si>
@@ -115,10 +115,10 @@
     <t>IMS-1M</t>
   </si>
   <si>
+    <t>to go</t>
+  </si>
+  <si>
     <t>https://aclanthology.coli.uni-saarland.de/papers/K15-1037/k15-1037.bib</t>
-  </si>
-  <si>
-    <t>to go</t>
   </si>
   <si>
     <t>paper</t>
@@ -191,6 +191,9 @@
     <t>c2v iters+</t>
   </si>
   <si>
+    <t>how to name systems</t>
+  </si>
+  <si>
     <t>context2vec</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
     <t>uns</t>
   </si>
   <si>
-    <t>how to name systems</t>
-  </si>
-  <si>
     <t>WSD-games</t>
   </si>
   <si>
@@ -233,34 +233,64 @@
     <t>games</t>
   </si>
   <si>
+    <t>higher than competition or close to</t>
+  </si>
+  <si>
     <t>IMS+embeddings</t>
   </si>
   <si>
+    <t>published results (not arxiv)</t>
+  </si>
+  <si>
     <t>https://aclanthology.coli.uni-saarland.de/papers/P16-1085/p16-1085.bib</t>
   </si>
   <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>-rag means raganato</t>
+  </si>
+  <si>
     <t>IMS-s+emb SemCor</t>
   </si>
   <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>best setting</t>
+  </si>
+  <si>
+    <t>all rag results are either from the paper or from raganato et al. (2017)</t>
+  </si>
+  <si>
+    <t>IMS+emb SemCor + OMSTI</t>
+  </si>
+  <si>
+    <t>IMS-s+emb SemCor + OMSTI</t>
+  </si>
+  <si>
     <t>Word2Vec OMSTI</t>
   </si>
   <si>
-    <t>IMS+emb SemCor + OMSTI</t>
-  </si>
-  <si>
     <t>IMS + Word2Vec (OMSTI)</t>
   </si>
   <si>
     <t>se2-aw___nouns</t>
   </si>
   <si>
-    <t>IMS-s+emb SemCor + OMSTI</t>
+    <t>IMS+emb (SemCor)</t>
   </si>
   <si>
     <t>IMS+emb SemCor</t>
   </si>
   <si>
-    <t>IMS+emb (SemCor)</t>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Training data</t>
+  </si>
+  <si>
+    <t>Domains_Supersenses</t>
   </si>
   <si>
     <t>IMS</t>
@@ -269,208 +299,43 @@
     <t>https://aclanthology.coli.uni-saarland.de/papers/P10-4014/p10-4014.bib</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>SC, DSO, MUN</t>
+  </si>
+  <si>
+    <t>Autoencoder</t>
+  </si>
+  <si>
+    <t>Google News</t>
+  </si>
+  <si>
+    <t>rank 1 system</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Dense subgraph</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>densest subgraph heuristic which selects high-coherence semantic interpretations.</t>
+  </si>
+  <si>
     <t>SemCor + OMSTI</t>
   </si>
   <si>
-    <t>rank 1 system</t>
-  </si>
-  <si>
-    <t>Google-LSTM</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/C16-1130/c16-1130.bib</t>
-  </si>
-  <si>
-    <t>LP T:SemCor, U:1K</t>
-  </si>
-  <si>
-    <t>higher than competition or close to</t>
-  </si>
-  <si>
-    <t>published results (not arxiv)</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>-rag means raganato</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>best setting</t>
-  </si>
-  <si>
-    <t>all rag results are either from the paper or from raganato et al. (2017)</t>
-  </si>
-  <si>
-    <t>LP T:OMSTI, U:1K</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>T:SemCor</t>
-  </si>
-  <si>
-    <t>Training data</t>
-  </si>
-  <si>
-    <t>Domains_Supersenses</t>
-  </si>
-  <si>
-    <t>se15-aw</t>
-  </si>
-  <si>
-    <t>LP T:SemCor, U:OMSTI</t>
-  </si>
-  <si>
-    <t>UKB</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/J14-1003/j14-1003.bib</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>SC, DSO, MUN</t>
-  </si>
-  <si>
-    <t>Nasari</t>
-  </si>
-  <si>
-    <t>https://scholar.googleusercontent.com/scholar.bib?q=info:L7bpWhZnosIJ:scholar.google.com/&amp;output=citation&amp;scisig=AAGBfm0AAAAAW3aYLyb7UeQ3P2UTiNSl6Loy7yZruaM8&amp;scisf=4&amp;ct=citation&amp;cd=-1&amp;hl=nl</t>
-  </si>
-  <si>
-    <t>lexical</t>
-  </si>
-  <si>
-    <t>Autoencoder</t>
-  </si>
-  <si>
-    <t>Google News</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>lexical +IMS</t>
-  </si>
-  <si>
-    <t>Dense subgraph</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t>LSTM</t>
   </si>
   <si>
     <t>SC, MUN</t>
-  </si>
-  <si>
-    <t>Multi-Objective Optimization</t>
-  </si>
-  <si>
-    <t>lexical + IMS</t>
-  </si>
-  <si>
-    <t>Attentive Bidirectional LSTM</t>
-  </si>
-  <si>
-    <t>SVM + embeddings</t>
-  </si>
-  <si>
-    <t>ukWaC</t>
-  </si>
-  <si>
-    <t>n,v,ar</t>
-  </si>
-  <si>
-    <t>gloss</t>
-  </si>
-  <si>
-    <t>Game-theoric</t>
-  </si>
-  <si>
-    <t>BLSTM + att</t>
-  </si>
-  <si>
-    <t>BLSTM + att + LEX</t>
-  </si>
-  <si>
-    <t>PPR</t>
-  </si>
-  <si>
-    <t>Neural-Sequence</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-1120/d17-1120.bib</t>
-  </si>
-  <si>
-    <t>BLSTM + att + LEX + POS</t>
-  </si>
-  <si>
-    <t>SMUaw</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/S01-1031/s01-1031.bib</t>
-  </si>
-  <si>
-    <t>SupWSD</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-2018/d17-2018.bib</t>
-  </si>
-  <si>
-    <t>SUPWSD+emb SemCor + OMSTI</t>
-  </si>
-  <si>
-    <t>SUPWSD+emb (SemCor + OMSTI)</t>
-  </si>
-  <si>
-    <t>se3-aw-rag</t>
-  </si>
-  <si>
-    <t>se7-aw-rag</t>
-  </si>
-  <si>
-    <t>se15-aw-rag</t>
-  </si>
-  <si>
-    <t>WSD-RNN</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/R17-2004/r17-2004.bib</t>
-  </si>
-  <si>
-    <t>Train-O-Matic Wiki</t>
-  </si>
-  <si>
-    <t>BabelNet</t>
-  </si>
-  <si>
-    <t>IMSeurosense</t>
-  </si>
-  <si>
-    <t>Train-O-Matic</t>
-  </si>
-  <si>
-    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-1008/d17-1008.bib</t>
-  </si>
-  <si>
-    <t>PPRw2w</t>
-  </si>
-  <si>
-    <t>static</t>
-  </si>
-  <si>
-    <t>densest subgraph heuristic which selects high-coherence semantic interpretations.</t>
   </si>
   <si>
     <t>for each concept: semantic signature</t>
@@ -482,7 +347,28 @@
 previously-computed semantic signatures. </t>
   </si>
   <si>
+    <t>Multi-Objective Optimization</t>
+  </si>
+  <si>
+    <t>Attentive Bidirectional LSTM</t>
+  </si>
+  <si>
+    <t>SVM + embeddings</t>
+  </si>
+  <si>
     <t>similar to Babelfy, but in a continuous setting</t>
+  </si>
+  <si>
+    <t>ukWaC</t>
+  </si>
+  <si>
+    <t>n,v,ar</t>
+  </si>
+  <si>
+    <t>Game-theoric</t>
+  </si>
+  <si>
+    <t>static</t>
   </si>
   <si>
     <t>context independent ranking of senses</t>
@@ -504,58 +390,205 @@
 nodes</t>
   </si>
   <si>
+    <t xml:space="preserve"> word-to-word -&gt; run ppr separately for each target word (no interaction with other target words)</t>
+  </si>
+  <si>
+    <t>PPR</t>
+  </si>
+  <si>
+    <t>iteratively updating graph when disambiguating (not with great results)</t>
+  </si>
+  <si>
+    <t>terminology</t>
+  </si>
+  <si>
+    <t>Google-LSTM</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/C16-1130/c16-1130.bib</t>
+  </si>
+  <si>
+    <t>sense</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>building matrices to achieve textual coherence (some words are more relevant than other for disambiguation)</t>
+  </si>
+  <si>
+    <t>LP T:OMSTI, U:1K</t>
+  </si>
+  <si>
+    <t>automatic mapping WordNet and Wikipedia</t>
+  </si>
+  <si>
+    <t>noun relations are transferred from Wikipedia to WordNet</t>
+  </si>
+  <si>
+    <t>WSD improves (on nouns) when doing this (e.g. more relatedness edges is better)</t>
+  </si>
+  <si>
+    <t>LP T:SemCor, U:1K</t>
+  </si>
+  <si>
+    <t>degee centrality</t>
+  </si>
+  <si>
+    <t>IDEA</t>
+  </si>
+  <si>
+    <t>can we add cross-pos relations automatically?</t>
+  </si>
+  <si>
+    <t>morphological normalization results</t>
+  </si>
+  <si>
+    <t>first sense way better connected than other senses</t>
+  </si>
+  <si>
+    <t>T:SemCor</t>
+  </si>
+  <si>
+    <t>Degree and PageRank good indication of hunger for knowledge</t>
+  </si>
+  <si>
+    <t>normalization and gloss relations extremely important</t>
+  </si>
+  <si>
+    <t>Degree or PR indication of hunger for knowledge</t>
+  </si>
+  <si>
+    <t>also use sense rank of indication of hunger for knowledge</t>
+  </si>
+  <si>
+    <t>se15-aw</t>
+  </si>
+  <si>
+    <t>LP T:SemCor, U:OMSTI</t>
+  </si>
+  <si>
+    <t>Nasari</t>
+  </si>
+  <si>
+    <t>https://scholar.googleusercontent.com/scholar.bib?q=info:L7bpWhZnosIJ:scholar.google.com/&amp;output=citation&amp;scisig=AAGBfm0AAAAAW3aYLyb7UeQ3P2UTiNSl6Loy7yZruaM8&amp;scisf=4&amp;ct=citation&amp;cd=-1&amp;hl=nl</t>
+  </si>
+  <si>
+    <t>lexical</t>
+  </si>
+  <si>
+    <t>lexical +IMS</t>
+  </si>
+  <si>
+    <t>lexical + IMS</t>
+  </si>
+  <si>
+    <t>WSD-RNN</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/R17-2004/r17-2004.bib</t>
+  </si>
+  <si>
+    <t>BLSTM + att</t>
+  </si>
+  <si>
+    <t>BLSTM + att + LEX</t>
+  </si>
+  <si>
+    <t>Neural-Sequence</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-1120/d17-1120.bib</t>
+  </si>
+  <si>
+    <t>BLSTM + att + LEX + POS</t>
+  </si>
+  <si>
+    <t>SMUaw</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/S01-1031/s01-1031.bib</t>
+  </si>
+  <si>
+    <t>context2vec already used knn</t>
+  </si>
+  <si>
+    <t>LIA-Sinequa</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/S01-1016/s01-1016.bib</t>
+  </si>
+  <si>
+    <t>SupWSD</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-2018/d17-2018.bib</t>
+  </si>
+  <si>
+    <t>SUPWSD+emb SemCor + OMSTI</t>
+  </si>
+  <si>
+    <t>SUPWSD+emb (SemCor + OMSTI)</t>
+  </si>
+  <si>
+    <t>se3-aw-rag</t>
+  </si>
+  <si>
+    <t>se7-aw-rag</t>
+  </si>
+  <si>
+    <t>se15-aw-rag</t>
+  </si>
+  <si>
+    <t>Train-O-Matic Wiki</t>
+  </si>
+  <si>
+    <t>BabelNet</t>
+  </si>
+  <si>
+    <t>IMSeurosense</t>
+  </si>
+  <si>
+    <t>Train-O-Matic</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/D17-1008/d17-1008.bib</t>
+  </si>
+  <si>
+    <t>UKB</t>
+  </si>
+  <si>
+    <t>https://aclanthology.coli.uni-saarland.de/papers/J14-1003/j14-1003.bib</t>
+  </si>
+  <si>
+    <t>gloss</t>
+  </si>
+  <si>
+    <t>PPRw2w</t>
+  </si>
+  <si>
     <t>UKB-optimal</t>
   </si>
   <si>
-    <t xml:space="preserve"> word-to-word -&gt; run ppr separately for each target word (no interaction with other target words)</t>
-  </si>
-  <si>
     <t>https://aclanthology.coli.uni-saarland.de/papers/W18-2505/w18-2505.bib</t>
   </si>
   <si>
-    <t>context2vec already used knn</t>
-  </si>
-  <si>
-    <t>iteratively updating graph when disambiguating (not with great results)</t>
-  </si>
-  <si>
-    <t>terminology</t>
-  </si>
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>player</t>
-  </si>
-  <si>
-    <t>sense</t>
-  </si>
-  <si>
-    <t>strategy</t>
-  </si>
-  <si>
     <t>UMCC-DLSI</t>
   </si>
   <si>
     <t>https://aclanthology.coli.uni-saarland.de/papers/S13-2042/s13-2042.bib</t>
   </si>
   <si>
-    <t>building matrices to achieve textual coherence (some words are more relevant than other for disambiguation)</t>
-  </si>
-  <si>
     <t>RUN-2</t>
   </si>
   <si>
-    <t>automatic mapping WordNet and Wikipedia</t>
-  </si>
-  <si>
     <t>WSD-TM</t>
-  </si>
-  <si>
-    <t>noun relations are transferred from Wikipedia to WordNet</t>
-  </si>
-  <si>
-    <t>WSD improves (on nouns) when doing this (e.g. more relatedness edges is better)</t>
   </si>
   <si>
     <t>@paper{AAAI1817415,
@@ -567,33 +600,6 @@
         abstract = {Word Sense Disambiguation is an open problem in Natural Language Processing which is particularly challenging and useful in the unsupervised setting where all the words in any given text need to be disambiguated without using any labeled data. Typically WSD systems use the sentence or a small window of words around the target word as the context for disambiguation because their computational complexity scales exponentially with the size of the context. In this paper, we leverage the formalism of topic model to design a WSD system that scales linearly with the number of words in the context. As a result, our system is able to utilize the whole document as the context for a word to be disambiguated. The proposed method is a variant of Latent Dirichlet Allocation in which the topic proportions for a document are replaced by synset proportions. We further utilize the information in the WordNet by assigning a non-uniform prior to synset distribution over words and a logistic-normal prior for document distribution over synsets. We evaluate the proposed method on Senseval-2, Senseval-3, SemEval-2007, SemEval-2013 and SemEval-2015 English All-Word WSD datasets and show that it outperforms the state-of-the-art unsupervised knowledge-based WSD system by a significant margin.},
         url = {https://aaai.org/ocs/index.php/AAAI/AAAI18/paper/view/17415/16787}
 }</t>
-  </si>
-  <si>
-    <t>degee centrality</t>
-  </si>
-  <si>
-    <t>IDEA</t>
-  </si>
-  <si>
-    <t>can we add cross-pos relations automatically?</t>
-  </si>
-  <si>
-    <t>morphological normalization results</t>
-  </si>
-  <si>
-    <t>first sense way better connected than other senses</t>
-  </si>
-  <si>
-    <t>Degree and PageRank good indication of hunger for knowledge</t>
-  </si>
-  <si>
-    <t>normalization and gloss relations extremely important</t>
-  </si>
-  <si>
-    <t>Degree or PR indication of hunger for knowledge</t>
-  </si>
-  <si>
-    <t>also use sense rank of indication of hunger for knowledge</t>
   </si>
 </sst>
 </file>
@@ -883,7 +889,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>33</v>
@@ -1284,10 +1290,10 @@
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>49</v>
@@ -1302,7 +1308,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>51</v>
@@ -1326,10 +1332,10 @@
         <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>49</v>
@@ -1344,7 +1350,7 @@
         <v>24</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>50</v>
@@ -1368,10 +1374,10 @@
         <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>49</v>
@@ -1386,7 +1392,7 @@
         <v>24</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>51</v>
@@ -1410,10 +1416,10 @@
         <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>49</v>
@@ -1428,7 +1434,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>50</v>
@@ -1458,7 +1464,7 @@
         <v>24</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>44</v>
@@ -1522,7 +1528,7 @@
         <v>24</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>47</v>
@@ -1580,10 +1586,10 @@
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>33</v>
@@ -1598,7 +1604,7 @@
         <v>24</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>46</v>
@@ -1625,13 +1631,13 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>26</v>
@@ -1655,13 +1661,13 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>26</v>
@@ -1691,7 +1697,7 @@
         <v>24</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>28</v>
@@ -1721,7 +1727,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>28</v>
@@ -1757,19 +1763,19 @@
         <v>2017.0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="N28" s="1">
-        <v>66.0</v>
+        <v>70.8</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>22</v>
@@ -1799,19 +1805,19 @@
         <v>2017.0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="N29" s="1">
-        <v>70.8</v>
+        <v>66.0</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>22</v>
@@ -1829,10 +1835,10 @@
         <v>22</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>49</v>
@@ -1847,7 +1853,7 @@
         <v>24</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>51</v>
@@ -1871,13 +1877,13 @@
         <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G31" s="1">
         <v>2016.0</v>
@@ -1889,19 +1895,17 @@
         <v>24</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="N31" s="1">
-        <v>68.3</v>
+        <v>66.3</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="R31" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="Q31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="str">
@@ -1915,10 +1919,10 @@
         <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>49</v>
@@ -1933,13 +1937,13 @@
         <v>24</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N32" s="1">
-        <v>70.8</v>
+        <v>66.7</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -1957,13 +1961,13 @@
         <v>22</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G33" s="1">
         <v>2016.0</v>
@@ -1975,17 +1979,19 @@
         <v>24</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="N33" s="1">
-        <v>66.3</v>
+        <v>68.3</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="R33" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="34" hidden="1">
       <c r="A34" s="3" t="str">
@@ -2005,7 +2011,7 @@
         <v>24</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>28</v>
@@ -2037,7 +2043,7 @@
         <v>24</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>47</v>
@@ -2069,10 +2075,10 @@
         <v>24</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="N36" s="1">
         <v>77.7</v>
@@ -2101,7 +2107,7 @@
         <v>24</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>44</v>
@@ -2133,7 +2139,7 @@
         <v>24</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>26</v>
@@ -2159,10 +2165,10 @@
         <v>22</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>49</v>
@@ -2177,13 +2183,13 @@
         <v>24</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N39" s="1">
-        <v>66.7</v>
+        <v>70.8</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -2201,10 +2207,10 @@
         <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>49</v>
@@ -2219,13 +2225,13 @@
         <v>24</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N40" s="1">
-        <v>71.0</v>
+        <v>67.3</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2243,10 +2249,10 @@
         <v>22</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>49</v>
@@ -2261,13 +2267,13 @@
         <v>24</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N41" s="1">
-        <v>72.2</v>
+        <v>71.0</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2285,10 +2291,10 @@
         <v>22</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>49</v>
@@ -2303,13 +2309,13 @@
         <v>24</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N42" s="1">
-        <v>73.3</v>
+        <v>72.2</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -2327,10 +2333,10 @@
         <v>22</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>49</v>
@@ -2345,13 +2351,13 @@
         <v>24</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N43" s="1">
-        <v>67.3</v>
+        <v>73.3</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -2369,10 +2375,10 @@
         <v>22</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>49</v>
@@ -2387,13 +2393,13 @@
         <v>24</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N44" s="1">
-        <v>65.0</v>
+        <v>70.9</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -2411,13 +2417,13 @@
         <v>22</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G45" s="1">
         <v>2010.0</v>
@@ -2429,13 +2435,13 @@
         <v>24</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N45" s="1">
-        <v>65.3</v>
+        <v>35</v>
+      </c>
+      <c r="M45" s="1">
+        <v>69.0</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
@@ -2453,10 +2459,10 @@
         <v>22</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>49</v>
@@ -2471,13 +2477,13 @@
         <v>24</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N46" s="1">
-        <v>70.9</v>
+        <v>72.8</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -2495,13 +2501,13 @@
         <v>22</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G47" s="1">
         <v>2010.0</v>
@@ -2513,13 +2519,13 @@
         <v>24</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M47" s="1">
-        <v>69.0</v>
+        <v>51</v>
+      </c>
+      <c r="N47" s="1">
+        <v>65.0</v>
       </c>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
@@ -2537,10 +2543,10 @@
         <v>22</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>49</v>
@@ -2555,13 +2561,13 @@
         <v>24</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N48" s="1">
-        <v>72.8</v>
+        <v>65.3</v>
       </c>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
@@ -2583,7 +2589,7 @@
         <v>24</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>28</v>
@@ -2611,7 +2617,7 @@
         <v>24</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>26</v>
@@ -2625,7 +2631,7 @@
     </row>
     <row r="51">
       <c r="A51" s="3" t="str">
-        <f t="shared" ref="A51:A57" si="10">HYPERLINK("http://aclweb.org/anthology/C16-1130","LSTM")</f>
+        <f t="shared" ref="A51:A58" si="10">HYPERLINK("http://aclweb.org/anthology/C16-1130","LSTM")</f>
         <v>LSTM</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2635,10 +2641,10 @@
         <v>22</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>33</v>
@@ -2653,13 +2659,13 @@
         <v>24</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="N51" s="1">
-        <v>69.5</v>
+        <v>74.4</v>
       </c>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -2685,7 +2691,7 @@
         <v>24</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>28</v>
@@ -2717,10 +2723,10 @@
         <v>24</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="N53" s="1">
         <v>79.9</v>
@@ -2749,7 +2755,7 @@
         <v>24</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>47</v>
@@ -2781,10 +2787,10 @@
         <v>24</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="N55" s="1">
         <v>72.6</v>
@@ -2813,7 +2819,7 @@
         <v>24</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>44</v>
@@ -2845,7 +2851,7 @@
         <v>24</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>26</v>
@@ -2861,8 +2867,8 @@
     </row>
     <row r="58">
       <c r="A58" s="3" t="str">
-        <f>HYPERLINK("http://aclweb.org/anthology/J14-1003","UKB")</f>
-        <v>UKB</v>
+        <f t="shared" si="10"/>
+        <v>LSTM</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>29</v>
@@ -2871,16 +2877,16 @@
         <v>22</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G58" s="1">
-        <v>2014.0</v>
+        <v>2016.0</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>23</v>
@@ -2888,11 +2894,19 @@
       <c r="I58" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J58" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="K58" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N58" s="1">
-        <v>56.0</v>
+        <v>69.5</v>
+      </c>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="59">
@@ -2907,10 +2921,10 @@
         <v>22</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>33</v>
@@ -2925,7 +2939,7 @@
         <v>24</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>46</v>
@@ -2958,7 +2972,7 @@
         <v>24</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>47</v>
@@ -2991,7 +3005,7 @@
         <v>24</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>47</v>
@@ -3018,10 +3032,10 @@
         <v>22</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>33</v>
@@ -3036,7 +3050,7 @@
         <v>24</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>46</v>
@@ -3052,9 +3066,9 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="str">
-        <f>HYPERLINK("http://aclweb.org/anthology/J14-1003","UKB")</f>
-        <v>UKB</v>
+      <c r="A63" s="4" t="str">
+        <f>HYPERLINK("http://www.acl-bg.org/proceedings/2017/RANLPStud%202017/pdf/RANLPStud004.pdf","Popov")</f>
+        <v>Popov</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>29</v>
@@ -3063,16 +3077,16 @@
         <v>22</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G63" s="1">
-        <v>2014.0</v>
+        <v>2017.0</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>23</v>
@@ -3081,13 +3095,13 @@
         <v>24</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N63" s="1">
-        <v>60.6</v>
+        <v>70.11</v>
       </c>
     </row>
     <row r="64" hidden="1">
@@ -3108,7 +3122,7 @@
         <v>24</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>28</v>
@@ -3137,10 +3151,10 @@
         <v>24</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="N65" s="1">
         <v>72.4</v>
@@ -3150,7 +3164,7 @@
     </row>
     <row r="66">
       <c r="A66" s="3" t="str">
-        <f>HYPERLINK("http://aclweb.org/anthology/D17-1120","Raganato_et_al_2017")</f>
+        <f t="shared" ref="A66:A67" si="13">HYPERLINK("http://aclweb.org/anthology/D17-1120","Raganato_et_al_2017")</f>
         <v>Raganato_et_al_2017</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -3160,10 +3174,10 @@
         <v>22</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>33</v>
@@ -3178,21 +3192,21 @@
         <v>24</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N66" s="1">
-        <v>66.9</v>
+        <v>72.0</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="str">
-        <f>HYPERLINK("http://aclweb.org/anthology/C16-1130","LSTM")</f>
-        <v>LSTM</v>
+        <f t="shared" si="13"/>
+        <v>Raganato_et_al_2017</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>29</v>
@@ -3201,16 +3215,16 @@
         <v>22</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G67" s="1">
-        <v>2016.0</v>
+        <v>2017.0</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>23</v>
@@ -3219,19 +3233,16 @@
         <v>24</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N67" s="1">
-        <v>74.4</v>
+        <v>66.9</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
-      <c r="Q67" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="4" t="str">
@@ -3245,10 +3256,10 @@
         <v>22</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>33</v>
@@ -3272,32 +3283,32 @@
         <v>69.0</v>
       </c>
       <c r="N68">
-        <f>(2 * (L68*M68)) / (L68+M68)</f>
+        <f t="shared" ref="N68:N69" si="14">(2 * (L68*M68)) / (L68+M68)</f>
         <v>69</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="str">
-        <f t="shared" ref="A69:A72" si="13">HYPERLINK("http://www.aclweb.org/anthology/D17-2018","SUP WSD")</f>
-        <v>SUP WSD</v>
+      <c r="A69" s="3" t="str">
+        <f>HYPERLINK("http://aclweb.org/anthology/S01-1016","LIA-Sinequa")</f>
+        <v>LIA-Sinequa</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G69" s="1">
-        <v>2017.0</v>
+        <v>2001.0</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>23</v>
@@ -3305,26 +3316,41 @@
       <c r="I69" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="J69" s="1"/>
       <c r="K69" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N69" s="1">
-        <v>67.2</v>
-      </c>
-    </row>
-    <row r="70" hidden="1">
+        <v>35</v>
+      </c>
+      <c r="L69" s="1">
+        <v>61.8</v>
+      </c>
+      <c r="M69" s="1">
+        <v>61.8</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="14"/>
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="70">
       <c r="A70" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="A70:A74" si="15">HYPERLINK("http://www.aclweb.org/anthology/D17-2018","SUP WSD")</f>
         <v>SUP WSD</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="B70" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G70" s="1">
         <v>2017.0</v>
       </c>
@@ -3335,18 +3361,18 @@
         <v>24</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>134</v>
+        <v>50</v>
       </c>
       <c r="N70" s="1">
-        <v>70.8</v>
+        <v>73.8</v>
       </c>
     </row>
     <row r="71" hidden="1">
       <c r="A71" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>SUP WSD</v>
       </c>
       <c r="B71" s="1"/>
@@ -3364,18 +3390,18 @@
         <v>24</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="N71" s="1">
-        <v>64.2</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="72" hidden="1">
       <c r="A72" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>SUP WSD</v>
       </c>
       <c r="B72" s="1"/>
@@ -3393,35 +3419,25 @@
         <v>24</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="N72" s="1">
-        <v>71.5</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="73" hidden="1">
       <c r="A73" s="4" t="str">
-        <f>HYPERLINK("http://www.acl-bg.org/proceedings/2017/RANLPStud%202017/pdf/RANLPStud004.pdf","Popov")</f>
-        <v>Popov</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>33</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>SUP WSD</v>
+      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
       <c r="G73" s="1">
         <v>2017.0</v>
       </c>
@@ -3432,25 +3448,35 @@
         <v>24</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="N73" s="1">
-        <v>70.11</v>
-      </c>
-    </row>
-    <row r="74" hidden="1">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="74">
       <c r="A74" s="4" t="str">
-        <f t="shared" ref="A74:A76" si="14">HYPERLINK("http://www.aclweb.org/anthology/D17-1008","Train-O-Matic")</f>
-        <v>Train-O-Matic</v>
-      </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+        <f t="shared" si="15"/>
+        <v>SUP WSD</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G74" s="1">
         <v>2017.0</v>
       </c>
@@ -3461,18 +3487,18 @@
         <v>24</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="N74" s="1">
-        <v>68.8</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="75" hidden="1">
       <c r="A75" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="A75:A77" si="16">HYPERLINK("http://www.aclweb.org/anthology/D17-1008","Train-O-Matic")</f>
         <v>Train-O-Matic</v>
       </c>
       <c r="B75" s="1"/>
@@ -3490,18 +3516,18 @@
         <v>24</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="N75" s="1">
-        <v>59.8</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="76" hidden="1">
       <c r="A76" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Train-O-Matic</v>
       </c>
       <c r="B76" s="1"/>
@@ -3519,19 +3545,19 @@
         <v>24</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="N76" s="1">
-        <v>67.4</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="77" hidden="1">
       <c r="A77" s="4" t="str">
-        <f t="shared" ref="A77:A78" si="15">HYPERLINK("http://www.aclweb.org/anthology/P17-2094","Eurosense")</f>
-        <v>Eurosense</v>
+        <f t="shared" si="16"/>
+        <v>Train-O-Matic</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3545,21 +3571,21 @@
         <v>23</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="N77" s="1">
-        <v>66.4</v>
+        <v>67.4</v>
       </c>
     </row>
     <row r="78" hidden="1">
       <c r="A78" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="A78:A79" si="17">HYPERLINK("http://www.aclweb.org/anthology/P17-2094","Eurosense")</f>
         <v>Eurosense</v>
       </c>
       <c r="B78" s="1"/>
@@ -3574,38 +3600,28 @@
         <v>23</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>140</v>
+        <v>171</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="N78" s="1">
-        <v>69.5</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>66.4</v>
+      </c>
+    </row>
+    <row r="79" hidden="1">
       <c r="A79" s="4" t="str">
-        <f>HYPERLINK("http://www.aclweb.org/anthology/D17-1008","Train-O-Matic")</f>
-        <v>Train-O-Matic</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>33</v>
-      </c>
+        <f t="shared" si="17"/>
+        <v>Eurosense</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
       <c r="G79" s="1">
         <v>2017.0</v>
       </c>
@@ -3613,22 +3629,22 @@
         <v>23</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="N79" s="1">
-        <v>65.5</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="3" t="str">
-        <f>HYPERLINK("http://aclweb.org/anthology/D17-1120","Raganato_et_al_2017")</f>
-        <v>Raganato_et_al_2017</v>
+      <c r="A80" s="4" t="str">
+        <f t="shared" ref="A80:A81" si="18">HYPERLINK("http://www.aclweb.org/anthology/D17-1008","Train-O-Matic")</f>
+        <v>Train-O-Matic</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>29</v>
@@ -3637,10 +3653,10 @@
         <v>22</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>33</v>
@@ -3655,21 +3671,19 @@
         <v>24</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N80" s="1">
-        <v>72.0</v>
-      </c>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
+        <v>70.5</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="3" t="str">
-        <f t="shared" ref="A81:A88" si="16">HYPERLINK("http://aclweb.org/anthology/J14-1003","UKB")</f>
-        <v>UKB</v>
+      <c r="A81" s="4" t="str">
+        <f t="shared" si="18"/>
+        <v>Train-O-Matic</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>29</v>
@@ -3678,16 +3692,16 @@
         <v>22</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>99</v>
+        <v>174</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G81" s="1">
-        <v>2014.0</v>
+        <v>2017.0</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>23</v>
@@ -3696,18 +3710,18 @@
         <v>24</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="N81" s="1">
-        <v>59.7</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="A82:A91" si="19">HYPERLINK("http://aclweb.org/anthology/J14-1003","UKB")</f>
         <v>UKB</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -3717,10 +3731,10 @@
         <v>22</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>49</v>
@@ -3735,15 +3749,15 @@
         <v>24</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N82" s="1">
-        <v>53.6</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -3753,10 +3767,10 @@
         <v>22</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>49</v>
@@ -3771,26 +3785,38 @@
         <v>24</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N83" s="1">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="84" hidden="1">
+        <v>60.6</v>
+      </c>
+    </row>
+    <row r="84">
       <c r="A84" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G84" s="1">
+        <v>2014.0</v>
+      </c>
       <c r="H84" s="1" t="s">
         <v>23</v>
       </c>
@@ -3798,21 +3824,18 @@
         <v>24</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="N84" s="1">
-        <v>71.8</v>
-      </c>
-      <c r="O84" s="1"/>
-      <c r="P84" s="1"/>
-      <c r="Q84" s="1"/>
+        <v>59.7</v>
+      </c>
     </row>
     <row r="85" hidden="1">
       <c r="A85" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
       <c r="B85" s="1"/>
@@ -3828,13 +3851,13 @@
         <v>24</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="N85" s="1">
-        <v>57.9</v>
+        <v>71.8</v>
       </c>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -3842,7 +3865,7 @@
     </row>
     <row r="86" hidden="1">
       <c r="A86" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
       <c r="B86" s="1"/>
@@ -3858,13 +3881,13 @@
         <v>24</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="N86" s="1">
-        <v>65.3</v>
+        <v>57.9</v>
       </c>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
@@ -3872,7 +3895,7 @@
     </row>
     <row r="87" hidden="1">
       <c r="A87" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
       <c r="B87" s="1"/>
@@ -3888,13 +3911,13 @@
         <v>24</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="N87" s="1">
-        <v>43.0</v>
+        <v>65.3</v>
       </c>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
@@ -3902,7 +3925,7 @@
     </row>
     <row r="88" hidden="1">
       <c r="A88" s="3" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>UKB</v>
       </c>
       <c r="B88" s="1"/>
@@ -3918,41 +3941,29 @@
         <v>24</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="N88" s="1">
-        <v>56.0</v>
+        <v>43.0</v>
       </c>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89">
-      <c r="A89" s="4" t="str">
-        <f>HYPERLINK("http://www.aclweb.org/anthology/D17-2018","SUP WSD")</f>
-        <v>SUP WSD</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G89" s="1">
-        <v>2017.0</v>
-      </c>
+    <row r="89" hidden="1">
+      <c r="A89" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>UKB</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
       <c r="H89" s="1" t="s">
         <v>23</v>
       </c>
@@ -3960,19 +3971,22 @@
         <v>24</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N89" s="1">
-        <v>73.8</v>
-      </c>
+        <v>56.0</v>
+      </c>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="str">
-        <f>HYPERLINK("http://www.aclweb.org/anthology/D17-1008","Train-O-Matic")</f>
-        <v>Train-O-Matic</v>
+      <c r="A90" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>UKB</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>29</v>
@@ -3981,16 +3995,16 @@
         <v>22</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G90" s="1">
-        <v>2017.0</v>
+        <v>2014.0</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>23</v>
@@ -3998,20 +4012,17 @@
       <c r="I90" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J90" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="K90" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N90" s="1">
-        <v>70.5</v>
+        <v>53.6</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="4" t="str">
-        <f t="shared" ref="A91:A92" si="17">HYPERLINK("http://aclweb.org/anthology/W18-2505","UKB optimal")</f>
-        <v>UKB optimal</v>
+      <c r="A91" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>UKB</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>29</v>
@@ -4020,16 +4031,16 @@
         <v>22</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G91" s="1">
-        <v>2018.0</v>
+        <v>2014.0</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>23</v>
@@ -4037,16 +4048,19 @@
       <c r="I91" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J91" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="K91" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N91" s="1">
-        <v>68.8</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="4" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="A92:A93" si="20">HYPERLINK("http://aclweb.org/anthology/W18-2505","UKB optimal")</f>
         <v>UKB optimal</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -4056,10 +4070,10 @@
         <v>22</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>33</v>
@@ -4074,7 +4088,7 @@
         <v>24</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N92" s="1">
         <v>68.8</v>
@@ -4082,93 +4096,95 @@
     </row>
     <row r="93">
       <c r="A93" s="4" t="str">
+        <f t="shared" si="20"/>
+        <v>UKB optimal</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G93" s="1">
+        <v>2018.0</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N93" s="1">
+        <v>68.8</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="4" t="str">
         <f>HYPERLINK("http://www.aclweb.org/anthology/S13-2042","UMCC DLSI")</f>
         <v>UMCC DLSI</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G93" s="1">
-        <v>2013.0</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N93" s="1">
-        <v>64.7</v>
-      </c>
-    </row>
-    <row r="94" ht="27.0" customHeight="1">
-      <c r="A94" s="4" t="str">
-        <f t="shared" ref="A94:A95" si="18">HYPERLINK("https://www.semanticscholar.org/paper/Knowledge-based-Word-Sense-Disambiguation-using-Chaplot-Salakhutdinov/d64abf2b548d805dbcb3a5b457406809df9b2bc2/figure/1","WSD-TM")</f>
-        <v>WSD-TM</v>
-      </c>
       <c r="B94" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G94" s="1">
-        <v>2018.0</v>
+        <v>2013.0</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J94" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="K94" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N94" s="1">
-        <v>65.3</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="95" ht="27.0" customHeight="1">
       <c r="A95" s="4" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="A95:A96" si="21">HYPERLINK("https://www.semanticscholar.org/paper/Knowledge-based-Word-Sense-Disambiguation-using-Chaplot-Salakhutdinov/d64abf2b548d805dbcb3a5b457406809df9b2bc2/figure/1","WSD-TM")</f>
         <v>WSD-TM</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C95" s="1"/>
+      <c r="C95" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D95" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>33</v>
@@ -4183,15 +4199,49 @@
         <v>24</v>
       </c>
       <c r="K95" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N95" s="1">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4" t="str">
+        <f t="shared" si="21"/>
+        <v>WSD-TM</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G96" s="1">
+        <v>2018.0</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K96" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N95" s="1">
+      <c r="N96" s="1">
         <v>69.0</v>
       </c>
     </row>
-    <row r="96" hidden="1"/>
+    <row r="97" hidden="1"/>
   </sheetData>
-  <autoFilter ref="$A$1:$S$96">
+  <autoFilter ref="$A$1:$S$97">
     <filterColumn colId="10">
       <filters>
         <filter val="se2-aw-v2"/>
@@ -4241,19 +4291,20 @@
     <hyperlink r:id="rId31" ref="E67"/>
     <hyperlink r:id="rId32" ref="E68"/>
     <hyperlink r:id="rId33" ref="E69"/>
-    <hyperlink r:id="rId34" ref="E73"/>
-    <hyperlink r:id="rId35" ref="E79"/>
+    <hyperlink r:id="rId34" ref="E70"/>
+    <hyperlink r:id="rId35" ref="E74"/>
     <hyperlink r:id="rId36" ref="E80"/>
     <hyperlink r:id="rId37" ref="E81"/>
     <hyperlink r:id="rId38" ref="E82"/>
     <hyperlink r:id="rId39" ref="E83"/>
-    <hyperlink r:id="rId40" ref="E89"/>
+    <hyperlink r:id="rId40" ref="E84"/>
     <hyperlink r:id="rId41" ref="E90"/>
     <hyperlink r:id="rId42" ref="E91"/>
     <hyperlink r:id="rId43" ref="E92"/>
     <hyperlink r:id="rId44" ref="E93"/>
+    <hyperlink r:id="rId45" ref="E94"/>
   </hyperlinks>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
 
@@ -4308,7 +4359,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <f>COUNTBLANK(C2:C22)</f>
@@ -4646,7 +4697,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4677,7 +4728,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -4685,7 +4736,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -4693,7 +4744,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6">
@@ -4701,7 +4752,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
@@ -4709,7 +4760,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
@@ -4717,7 +4768,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -4725,7 +4776,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4761,37 +4812,37 @@
         <v>18</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("UNIQUE(results!A2:A70)"),"1million")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("UNIQUE(results!A2:A71)"),"1million")</f>
         <v>1million</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
@@ -4803,19 +4854,19 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -4827,19 +4878,19 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -4851,19 +4902,19 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
@@ -4875,19 +4926,19 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
@@ -4899,16 +4950,16 @@
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -4920,19 +4971,19 @@
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
@@ -4941,19 +4992,19 @@
         <v>DFKI</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
@@ -4965,19 +5016,19 @@
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
@@ -4989,19 +5040,19 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12">
@@ -5013,16 +5064,16 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -5034,16 +5085,16 @@
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
@@ -5054,14 +5105,14 @@
     </row>
     <row r="15">
       <c r="A15" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"UKB")</f>
-        <v>UKB</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Nasari")</f>
+        <v>Nasari</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Nasari")</f>
-        <v>Nasari</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Popov")</f>
+        <v>Popov</v>
       </c>
     </row>
     <row r="17">
@@ -5084,6 +5135,12 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"LIA-Sinequa")</f>
+        <v>LIA-Sinequa</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"SUP WSD")</f>
         <v>SUP WSD</v>
       </c>
@@ -5108,8 +5165,9 @@
     <hyperlink r:id="rId16" ref="A18"/>
     <hyperlink r:id="rId17" ref="A19"/>
     <hyperlink r:id="rId18" ref="A20"/>
+    <hyperlink r:id="rId19" ref="A21"/>
   </hyperlinks>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -5131,17 +5189,17 @@
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
@@ -5150,7 +5208,7 @@
         <v>DFKI</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6">
@@ -5161,18 +5219,18 @@
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9">
@@ -5180,7 +5238,7 @@
         <v>1.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10">
@@ -5188,7 +5246,7 @@
         <v>2.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="1">
@@ -5196,7 +5254,7 @@
         <v>3.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12">
@@ -5204,7 +5262,7 @@
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
@@ -5213,7 +5271,7 @@
         <v>SUDOKU</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
@@ -5222,28 +5280,28 @@
         <v>Game-theoretic</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="1" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="1" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18">
@@ -5257,7 +5315,7 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20">
@@ -5265,7 +5323,7 @@
         <v>2.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21">
@@ -5273,7 +5331,7 @@
         <v>3.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22">
@@ -5282,24 +5340,24 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="1" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24">
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -5314,7 +5372,7 @@
         <v>1.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27">
@@ -5322,7 +5380,7 @@
         <v>2.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
@@ -5330,31 +5388,31 @@
         <v>3.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="1" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="1" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -5377,7 +5435,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>